<commit_message>
Reduced verbosity to more easily identify False Negatives. Updated program to include information to more easily figure out False Positives. Added False Negative results in .xls file.
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="suj" sheetId="2" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="kaist" sheetId="5" r:id="rId7"/>
     <sheet name="3movie timings" sheetId="6" r:id="rId8"/>
     <sheet name="all" sheetId="9" r:id="rId9"/>
+    <sheet name="robust" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -171,6 +172,54 @@
     <t>Avg. luma dist</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>cif</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>qcif</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>brate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fps</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5fps</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 degree</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2 degree</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3 degree</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SUJ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KAIST</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Total comparisons</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +350,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -372,11 +420,11 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:axId val="95286400"/>
-        <c:axId val="96750208"/>
+        <c:axId val="87171072"/>
+        <c:axId val="87173376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95286400"/>
+        <c:axId val="87171072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,17 +446,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96750208"/>
+        <c:crossAx val="87173376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96750208"/>
+        <c:axId val="87173376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,11 +478,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95286400"/>
+        <c:crossAx val="87171072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -444,7 +490,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -807,11 +853,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95236480"/>
-        <c:axId val="94907008"/>
+        <c:axId val="88237568"/>
+        <c:axId val="88239488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95236480"/>
+        <c:axId val="88237568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -842,12 +888,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94907008"/>
+        <c:crossAx val="88239488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94907008"/>
+        <c:axId val="88239488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +920,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95236480"/>
+        <c:crossAx val="88237568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -887,7 +933,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1091,11 +1137,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="105820160"/>
-        <c:axId val="105822848"/>
+        <c:axId val="88266240"/>
+        <c:axId val="88268160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105820160"/>
+        <c:axId val="88266240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,14 +1170,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105822848"/>
+        <c:crossAx val="88268160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105822848"/>
+        <c:axId val="88268160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,7 +1204,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105820160"/>
+        <c:crossAx val="88266240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1171,7 +1217,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1283,11 +1329,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="66927232"/>
-        <c:axId val="66962176"/>
+        <c:axId val="79456512"/>
+        <c:axId val="79491456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66927232"/>
+        <c:axId val="79456512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,14 +1359,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66962176"/>
+        <c:crossAx val="79491456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66962176"/>
+        <c:axId val="79491456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,7 +1402,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66927232"/>
+        <c:crossAx val="79456512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1371,7 +1417,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1482,11 +1528,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67133824"/>
-        <c:axId val="67135744"/>
+        <c:axId val="87243776"/>
+        <c:axId val="87258624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67133824"/>
+        <c:axId val="87243776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1511,12 +1557,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67135744"/>
+        <c:crossAx val="87258624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67135744"/>
+        <c:axId val="87258624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1559,7 +1605,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67133824"/>
+        <c:crossAx val="87243776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1572,7 +1618,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1662,11 +1708,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="67340160"/>
-        <c:axId val="67346432"/>
+        <c:axId val="87716992"/>
+        <c:axId val="87718912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67340160"/>
+        <c:axId val="87716992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,17 +1734,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67346432"/>
+        <c:crossAx val="87718912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67346432"/>
+        <c:axId val="87718912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1720,11 +1765,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67340160"/>
+        <c:crossAx val="87716992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1733,7 +1777,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1823,11 +1867,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76276864"/>
-        <c:axId val="76278784"/>
+        <c:axId val="87739008"/>
+        <c:axId val="87622400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76276864"/>
+        <c:axId val="87739008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,17 +1893,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76278784"/>
+        <c:crossAx val="87622400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76278784"/>
+        <c:axId val="87622400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,11 +1924,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76276864"/>
+        <c:crossAx val="87739008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1894,7 +1936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1984,11 +2026,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60125568"/>
-        <c:axId val="60127488"/>
+        <c:axId val="87896448"/>
+        <c:axId val="87898368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60125568"/>
+        <c:axId val="87896448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,17 +2052,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60127488"/>
+        <c:crossAx val="87898368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60127488"/>
+        <c:axId val="87898368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,11 +2083,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60125568"/>
+        <c:crossAx val="87896448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2055,7 +2095,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2109,22 +2149,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="67366272"/>
-        <c:axId val="66598016"/>
+        <c:axId val="87910272"/>
+        <c:axId val="87911808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67366272"/>
+        <c:axId val="87910272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66598016"/>
+        <c:crossAx val="87911808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66598016"/>
+        <c:axId val="87911808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,20 +2172,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67366272"/>
+        <c:crossAx val="87910272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2408,11 +2447,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71510272"/>
-        <c:axId val="71520640"/>
+        <c:axId val="88019712"/>
+        <c:axId val="88021632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71510272"/>
+        <c:axId val="88019712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2439,12 +2478,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71520640"/>
+        <c:crossAx val="88021632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71520640"/>
+        <c:axId val="88021632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2471,7 +2510,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71510272"/>
+        <c:crossAx val="88019712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2490,7 +2529,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2838,11 +2877,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="56813824"/>
-        <c:axId val="60101376"/>
+        <c:axId val="88110208"/>
+        <c:axId val="88112128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56813824"/>
+        <c:axId val="88110208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2868,14 +2907,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60101376"/>
+        <c:crossAx val="88112128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60101376"/>
+        <c:axId val="88112128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,7 +2941,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56813824"/>
+        <c:crossAx val="88110208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2915,7 +2954,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3900,6 +3939,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="4" max="4" width="1.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>48400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>97</v>
+      </c>
+      <c r="E5">
+        <f>(B5-2)/(C2)</f>
+        <v>4.1322314049586776E-4</v>
+      </c>
+      <c r="F5">
+        <f>(C5-2)/(C2)</f>
+        <v>1.962809917355372E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>81</v>
+      </c>
+      <c r="E6">
+        <f>(B6-2)/(C2)</f>
+        <v>3.3057851239669424E-4</v>
+      </c>
+      <c r="F6">
+        <f>(C6-2)/(C2)</f>
+        <v>1.6322314049586777E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>93</v>
+      </c>
+      <c r="E7">
+        <f>(B7-2)/(C2)</f>
+        <v>1.2396694214876033E-4</v>
+      </c>
+      <c r="F7">
+        <f>(C7-2)/(C2)</f>
+        <v>1.8801652892561983E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>83</v>
+      </c>
+      <c r="E8">
+        <f>(B8-2)/(C2)</f>
+        <v>1.4462809917355373E-4</v>
+      </c>
+      <c r="F8">
+        <f>(C8-2)/(C2)</f>
+        <v>1.6735537190082645E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>98</v>
+      </c>
+      <c r="E9">
+        <f>(B9-2)/(C2)</f>
+        <v>5.7851239669421491E-4</v>
+      </c>
+      <c r="F9">
+        <f>(C9-2)/(C2)</f>
+        <v>1.9834710743801653E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <f>(B10-2)/(C2)</f>
+        <v>1.0743801652892562E-3</v>
+      </c>
+      <c r="F10">
+        <f>(C10-2)/(C2)</f>
+        <v>1.6115702479338842E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <f>(B11-2)/(C2)</f>
+        <v>3.3057851239669424E-4</v>
+      </c>
+      <c r="F11">
+        <f>(C11-2)/(C2)</f>
+        <v>1.7148760330578513E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>86</v>
+      </c>
+      <c r="E12">
+        <f>(B12-2)/(C2)</f>
+        <v>4.1322314049586776E-4</v>
+      </c>
+      <c r="F12">
+        <f>(C12-2)/(C2)</f>
+        <v>1.7355371900826446E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <f>(B13-2)/(C2)</f>
+        <v>4.5454545454545455E-4</v>
+      </c>
+      <c r="F13">
+        <f>(C13-2)/(C2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J39"/>
@@ -7136,8 +7389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
- Renamed the old videofingerprinting.c file to videofingerprinting_robust.c. That file will contain the robustness tests and KAISTs implementation. - The actual videofingerprinting.c is geared to a better integration with encluster3. - Updated the xls file to have a few more results
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -218,6 +218,10 @@
   </si>
   <si>
     <t>Total comparisons</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>False Positive SEGMENTS</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3941,10 +3945,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3952,20 +3956,29 @@
     <col min="4" max="4" width="1.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="C2">
         <v>48400</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <v>48400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -3978,8 +3991,20 @@
       <c r="F4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3997,8 +4022,22 @@
         <f>(C5-2)/(C2)</f>
         <v>1.962809917355372E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5">
+        <v>1381</v>
+      </c>
+      <c r="M5">
+        <f>(J5-2)/(K2)</f>
+        <v>2.8491735537190081E-2</v>
+      </c>
+      <c r="N5">
+        <f>(K5-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -4016,8 +4055,22 @@
         <f>(C6-2)/(C2)</f>
         <v>1.6322314049586777E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
+        <v>1429</v>
+      </c>
+      <c r="M6">
+        <f>(J6-2)/(K2)</f>
+        <v>2.9483471074380166E-2</v>
+      </c>
+      <c r="N6">
+        <f>(K6-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -4035,8 +4088,22 @@
         <f>(C7-2)/(C2)</f>
         <v>1.8801652892561983E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7">
+        <v>1436</v>
+      </c>
+      <c r="M7">
+        <f>(J7-2)/(K2)</f>
+        <v>2.9628099173553718E-2</v>
+      </c>
+      <c r="N7">
+        <f>(K7-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -4054,8 +4121,22 @@
         <f>(C8-2)/(C2)</f>
         <v>1.6735537190082645E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <v>1444</v>
+      </c>
+      <c r="M8">
+        <f>(J8-2)/(K2)</f>
+        <v>2.9793388429752068E-2</v>
+      </c>
+      <c r="N8">
+        <f>(K8-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -4073,8 +4154,22 @@
         <f>(C9-2)/(C2)</f>
         <v>1.9834710743801653E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9">
+        <v>935</v>
+      </c>
+      <c r="M9">
+        <f>(J9-2)/(K2)</f>
+        <v>1.9276859504132233E-2</v>
+      </c>
+      <c r="N9">
+        <f>(K9-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -4092,8 +4187,22 @@
         <f>(C10-2)/(C2)</f>
         <v>1.6115702479338842E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10">
+        <v>675</v>
+      </c>
+      <c r="M10">
+        <f>(J10-2)/(K2)</f>
+        <v>1.3904958677685951E-2</v>
+      </c>
+      <c r="N10">
+        <f>(K10-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -4111,8 +4220,22 @@
         <f>(C11-2)/(C2)</f>
         <v>1.7148760330578513E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11">
+        <v>1468</v>
+      </c>
+      <c r="M11">
+        <f>(J11-2)/(K2)</f>
+        <v>3.0289256198347107E-2</v>
+      </c>
+      <c r="N11">
+        <f>(K11-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -4130,13 +4253,30 @@
         <f>(C12-2)/(C2)</f>
         <v>1.7355371900826446E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12">
+        <v>1450</v>
+      </c>
+      <c r="M12">
+        <f>(J12-2)/(K2)</f>
+        <v>2.9917355371900826E-2</v>
+      </c>
+      <c r="N12">
+        <f>(K12-2)/(K2)</f>
+        <v>-4.132231404958678E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>45</v>
       </c>
       <c r="B13">
         <v>24</v>
+      </c>
+      <c r="C13">
+        <v>82</v>
       </c>
       <c r="E13">
         <f>(B13-2)/(C2)</f>
@@ -4144,6 +4284,20 @@
       </c>
       <c r="F13">
         <f>(C13-2)/(C2)</f>
+        <v>1.652892561983471E-3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13">
+        <v>1418</v>
+      </c>
+      <c r="M13">
+        <f>(J13-2)/(K2)</f>
+        <v>2.9256198347107437E-2</v>
+      </c>
+      <c r="N13">
+        <f>(K13-2)/(K2)</f>
         <v>-4.132231404958678E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated some graphs for the ISCIT/ICCE papers in the excel file. Minor fixes on code.
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -173,42 +173,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>cif</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>qcif</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>brate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>gray</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>fps</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5fps</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1 degree</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2 degree</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>3 degree</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>SUJ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -222,6 +186,56 @@
   </si>
   <si>
     <t>False Positive SEGMENTS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Resize to CIF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Resize to QCIF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lossy compression</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Grayscale conversion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rotation of 1 degree</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rotation of 2 degrees</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rotation of 3 degrees</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Frame-rate change
+ to 5 fps</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Frame-rate change
+to 15 fps</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Avg.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Avg. (without fps)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Avg. performance gain</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -282,12 +296,38 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -296,7 +336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -322,6 +362,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -424,11 +473,11 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:axId val="87171072"/>
-        <c:axId val="87173376"/>
+        <c:axId val="75417472"/>
+        <c:axId val="75436416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87171072"/>
+        <c:axId val="75417472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,14 +501,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87173376"/>
+        <c:crossAx val="75436416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87173376"/>
+        <c:axId val="75436416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +534,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87171072"/>
+        <c:crossAx val="75417472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -494,7 +543,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -857,11 +906,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="88237568"/>
-        <c:axId val="88239488"/>
+        <c:axId val="76668288"/>
+        <c:axId val="76674560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88237568"/>
+        <c:axId val="76668288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -888,16 +937,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88239488"/>
+        <c:crossAx val="76674560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88239488"/>
+        <c:axId val="76674560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,24 +968,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88237568"/>
+        <c:crossAx val="76668288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -964,7 +1010,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1141,11 +1186,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88266240"/>
-        <c:axId val="88268160"/>
+        <c:axId val="77749632"/>
+        <c:axId val="77760000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88266240"/>
+        <c:axId val="77749632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,17 +1216,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88268160"/>
+        <c:crossAx val="77760000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88268160"/>
+        <c:axId val="77760000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,24 +1248,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88266240"/>
+        <c:crossAx val="77749632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1333,11 +1375,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="79456512"/>
-        <c:axId val="79491456"/>
+        <c:axId val="76185984"/>
+        <c:axId val="76187904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79456512"/>
+        <c:axId val="76185984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,14 +1405,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79491456"/>
+        <c:crossAx val="76187904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79491456"/>
+        <c:axId val="76187904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1448,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79456512"/>
+        <c:crossAx val="76185984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,7 +1463,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1532,11 +1574,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="87243776"/>
-        <c:axId val="87258624"/>
+        <c:axId val="76203136"/>
+        <c:axId val="76205440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87243776"/>
+        <c:axId val="76203136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1561,12 +1603,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87258624"/>
+        <c:crossAx val="76205440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87258624"/>
+        <c:axId val="76205440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1609,7 +1651,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87243776"/>
+        <c:crossAx val="76203136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1622,7 +1664,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1712,11 +1754,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87716992"/>
-        <c:axId val="87718912"/>
+        <c:axId val="75557888"/>
+        <c:axId val="76223616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87716992"/>
+        <c:axId val="75557888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,13 +1783,13 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87718912"/>
+        <c:crossAx val="76223616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87718912"/>
+        <c:axId val="76223616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1814,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87716992"/>
+        <c:crossAx val="75557888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1781,7 +1823,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,11 +1913,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87739008"/>
-        <c:axId val="87622400"/>
+        <c:axId val="76247808"/>
+        <c:axId val="76249728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87739008"/>
+        <c:axId val="76247808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,13 +1942,13 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87622400"/>
+        <c:crossAx val="76249728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87622400"/>
+        <c:axId val="76249728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +1973,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87739008"/>
+        <c:crossAx val="76247808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1940,7 +1982,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2030,11 +2072,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87896448"/>
-        <c:axId val="87898368"/>
+        <c:axId val="76380416"/>
+        <c:axId val="76394880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87896448"/>
+        <c:axId val="76380416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2059,13 +2101,13 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87898368"/>
+        <c:crossAx val="76394880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87898368"/>
+        <c:axId val="76394880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2132,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87896448"/>
+        <c:crossAx val="76380416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2099,7 +2141,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2153,22 +2195,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87910272"/>
-        <c:axId val="87911808"/>
+        <c:axId val="76308480"/>
+        <c:axId val="76310016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87910272"/>
+        <c:axId val="76308480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87911808"/>
+        <c:crossAx val="76310016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87911808"/>
+        <c:axId val="76310016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2218,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87910272"/>
+        <c:crossAx val="76308480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2188,7 +2230,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2451,11 +2493,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="88019712"/>
-        <c:axId val="88021632"/>
+        <c:axId val="76589696"/>
+        <c:axId val="76448512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88019712"/>
+        <c:axId val="76589696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2478,16 +2520,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88021632"/>
+        <c:crossAx val="76448512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88021632"/>
+        <c:axId val="76448512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2510,18 +2551,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88019712"/>
+        <c:crossAx val="76589696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2533,7 +2572,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2560,7 +2599,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -2881,11 +2919,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88110208"/>
-        <c:axId val="88112128"/>
+        <c:axId val="76471296"/>
+        <c:axId val="76608640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88110208"/>
+        <c:axId val="76471296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2907,18 +2945,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88112128"/>
+        <c:crossAx val="76608640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88112128"/>
+        <c:axId val="76608640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,24 +2978,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88110208"/>
+        <c:crossAx val="76471296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3945,15 +3980,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="4" max="4" width="1.625" customWidth="1"/>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="2" max="3" width="9" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="1.625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="1.75" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3961,349 +4002,465 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>48400</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K2">
         <v>48400</v>
       </c>
     </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
     <row r="4" spans="1:14">
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" t="s">
-        <v>47</v>
+      <c r="A4" s="11"/>
+      <c r="B4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9">
         <v>22</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>97</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <f>(B5-2)/(C2)</f>
         <v>4.1322314049586776E-4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <f>(C5-2)/(C2)</f>
         <v>1.962809917355372E-3</v>
       </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5">
+      <c r="G5">
+        <f>(F5/E5)</f>
+        <v>4.7500000000000009</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="9">
         <v>1381</v>
       </c>
-      <c r="M5">
+      <c r="K5" s="9">
+        <v>78273</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9">
         <f>(J5-2)/(K2)</f>
         <v>2.8491735537190081E-2</v>
       </c>
-      <c r="N5">
-        <f>(K5-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N5" s="9">
+        <f>(K5-2)/(K2)/24</f>
+        <v>6.7382059228650135E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="9">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>81</v>
       </c>
-      <c r="E6">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
         <f>(B6-2)/(C2)</f>
         <v>3.3057851239669424E-4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <f>(C6-2)/(C2)</f>
         <v>1.6322314049586777E-3</v>
       </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6">
+      <c r="G6">
+        <f t="shared" ref="G6:G13" si="0">(F6/E6)</f>
+        <v>4.9375</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="9">
         <v>1429</v>
       </c>
-      <c r="M6">
+      <c r="K6" s="9">
+        <v>25704</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9">
         <f>(J6-2)/(K2)</f>
         <v>2.9483471074380166E-2</v>
       </c>
-      <c r="N6">
-        <f>(K6-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N6" s="9">
+        <f>(K6-2)/(K2)/24</f>
+        <v>2.2126377410468318E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="9">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>93</v>
       </c>
-      <c r="E7">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <f>(B7-2)/(C2)</f>
         <v>1.2396694214876033E-4</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <f>(C7-2)/(C2)</f>
         <v>1.8801652892561983E-3</v>
       </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>15.166666666666666</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="9">
         <v>1436</v>
       </c>
-      <c r="M7">
+      <c r="K7" s="9">
+        <v>70009</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9">
         <f>(J7-2)/(K2)</f>
         <v>2.9628099173553718E-2</v>
       </c>
-      <c r="N7">
-        <f>(K7-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N7" s="9">
+        <f>(K7-2)/(K2)/24</f>
+        <v>6.0267734159779617E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="9">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>83</v>
       </c>
-      <c r="E8">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <f>(B8-2)/(C2)</f>
         <v>1.4462809917355373E-4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <f>(C8-2)/(C2)</f>
         <v>1.6735537190082645E-3</v>
       </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>11.571428571428571</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="9">
         <v>1444</v>
       </c>
-      <c r="M8">
+      <c r="K8" s="9">
+        <v>76704</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9">
         <f>(J8-2)/(K2)</f>
         <v>2.9793388429752068E-2</v>
       </c>
-      <c r="N8">
-        <f>(K8-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9">
+      <c r="N8" s="9">
+        <f>(K8-2)/(K2)/24</f>
+        <v>6.6031336088154272E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="29.25" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="9">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>98</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <f>(B9-2)/(C2)</f>
         <v>5.7851239669421491E-4</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="9">
         <f>(C9-2)/(C2)</f>
         <v>1.9834710743801653E-3</v>
       </c>
-      <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="9">
         <v>935</v>
       </c>
-      <c r="M9">
+      <c r="K9" s="9">
+        <v>55621</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9">
         <f>(J9-2)/(K2)</f>
         <v>1.9276859504132233E-2</v>
       </c>
-      <c r="N9">
-        <f>(K9-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10">
+      <c r="N9" s="9">
+        <f>(K9-2)/(K2)/24</f>
+        <v>4.7881370523415977E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="29.25" customHeight="1">
+      <c r="A10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="9">
         <v>54</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>80</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <f>(B10-2)/(C2)</f>
         <v>1.0743801652892562E-3</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="9">
         <f>(C10-2)/(C2)</f>
         <v>1.6115702479338842E-3</v>
       </c>
-      <c r="I10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="9">
         <v>675</v>
       </c>
-      <c r="M10">
+      <c r="K10" s="9">
+        <v>38571</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9">
         <f>(J10-2)/(K2)</f>
         <v>1.3904958677685951E-2</v>
       </c>
-      <c r="N10">
-        <f>(K10-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N10" s="9">
+        <f>(K10-2)/(K2)/24</f>
+        <v>3.3203340220385673E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="9">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>85</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <f>(B11-2)/(C2)</f>
         <v>3.3057851239669424E-4</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <f>(C11-2)/(C2)</f>
         <v>1.7148760330578513E-3</v>
       </c>
-      <c r="I11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>5.1875</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="9">
         <v>1468</v>
       </c>
-      <c r="M11">
+      <c r="K11" s="9">
+        <v>85691</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9">
         <f>(J11-2)/(K2)</f>
         <v>3.0289256198347107E-2</v>
       </c>
-      <c r="N11">
-        <f>(K11-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N11" s="9">
+        <f>(K11-2)/(K2)/24</f>
+        <v>7.3768078512396695E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="9">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>86</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <f>(B12-2)/(C2)</f>
         <v>4.1322314049586776E-4</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <f>(C12-2)/(C2)</f>
         <v>1.7355371900826446E-3</v>
       </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="9">
         <v>1450</v>
       </c>
-      <c r="M12">
+      <c r="K12" s="9">
+        <v>81435</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9">
         <f>(J12-2)/(K2)</f>
         <v>2.9917355371900826E-2</v>
       </c>
-      <c r="N12">
-        <f>(K12-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N12" s="9">
+        <f>(K12-2)/(K2)/24</f>
+        <v>7.0104166666666676E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="9">
         <v>24</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>82</v>
       </c>
-      <c r="E13">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <f>(B13-2)/(C2)</f>
         <v>4.5454545454545455E-4</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <f>(C13-2)/(C2)</f>
         <v>1.652892561983471E-3</v>
       </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="9">
         <v>1418</v>
       </c>
-      <c r="M13">
+      <c r="K13" s="9">
+        <v>37160</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9">
         <f>(J13-2)/(K2)</f>
         <v>2.9256198347107437E-2</v>
       </c>
-      <c r="N13">
-        <f>(K13-2)/(K2)</f>
-        <v>-4.132231404958678E-5</v>
+      <c r="N13" s="9">
+        <f>(K13-2)/(K2)/24</f>
+        <v>3.1988636363636365E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G5:G13)</f>
+        <v>6.0420033670033666</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15">
+        <f>AVERAGE(M11:M13,M5:M8)</f>
+        <v>2.9551357733175916E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="I16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16">
+        <f>AVERAGE(M5:M13)</f>
+        <v>2.66712580348944E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixing .c files to run on mac, for some reason strrchr() is giving me a segfault. Updated to latest results on xls file. Improved .doc files.
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="suj" sheetId="2" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="3movie timings" sheetId="6" r:id="rId8"/>
     <sheet name="all" sheetId="9" r:id="rId9"/>
     <sheet name="robust" sheetId="10" r:id="rId10"/>
+    <sheet name="thresholds" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -238,12 +239,120 @@
     <t>Avg. performance gain</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>FP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hashthresh</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L1 (fps)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10x.xx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bthresh/bt_L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/0.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/0.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3/0.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5/0.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>15/1.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>15/1.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The bigger this threshold is, the more movies pass the L2 check.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In the algorithm, a higher difference between time indexes and its Luma values is allowed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The bigger this threshold is, the more movies pass the L1 check.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In the algorithm, more movies are selected to the following phases.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>For some reason, that does not vary as much as expected.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>What's up with 5/0.5?</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>l3fact</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The bigger this threshold is, more strict the algorithm is</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L3 (fps)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Time (s)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FPR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FNR</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +379,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -336,7 +453,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -372,6 +489,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,11 +602,11 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:axId val="75417472"/>
-        <c:axId val="75436416"/>
+        <c:axId val="61057280"/>
+        <c:axId val="61076224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75417472"/>
+        <c:axId val="61057280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,14 +630,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75436416"/>
+        <c:crossAx val="61076224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75436416"/>
+        <c:axId val="61076224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +663,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75417472"/>
+        <c:crossAx val="61057280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -543,7 +672,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -906,11 +1035,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="76668288"/>
-        <c:axId val="76674560"/>
+        <c:axId val="66449408"/>
+        <c:axId val="66451328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76668288"/>
+        <c:axId val="66449408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -937,15 +1066,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76674560"/>
+        <c:crossAx val="66451328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76674560"/>
+        <c:axId val="66451328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,22 +1098,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76668288"/>
+        <c:crossAx val="66449408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1010,6 +1142,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1023,12 +1156,51 @@
           <c:tx>
             <c:v>VectD</c:v>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>all!$B$17:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1063,6 +1235,42 @@
           <c:tx>
             <c:v>Half VectD</c:v>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>all!$B$18:$J$18</c:f>
@@ -1106,6 +1314,42 @@
           <c:tx>
             <c:v>Tanimoto</c:v>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>all!$B$19:$J$19</c:f>
@@ -1149,6 +1393,42 @@
           <c:tx>
             <c:v>Tight Tani</c:v>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>all!$B$20:$J$20</c:f>
@@ -1186,11 +1466,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77749632"/>
-        <c:axId val="77760000"/>
+        <c:axId val="66490368"/>
+        <c:axId val="66492288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77749632"/>
+        <c:axId val="66490368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1216,16 +1496,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77760000"/>
+        <c:crossAx val="66492288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77760000"/>
+        <c:axId val="66492288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,22 +1530,1016 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77749632"/>
+        <c:crossAx val="66490368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>False Negatives</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>VectD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>all!$B$17:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tanimoto</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>all!$B$19:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="42851328"/>
+        <c:axId val="42861696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="42851328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>DB</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" baseline="0"/>
+                  <a:t> Threshold</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42861696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42861696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>Hits</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42851328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>False Positives</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>VectD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>all!$B$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tanimoto</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>all!$B$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>all!$B$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="78793344"/>
+        <c:axId val="81773312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="78793344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DB Threshold</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81773312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="81773312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hits</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78793344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>VectD</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="F79646">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>all!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>all!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>67.150000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tanimoto</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>all!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>all!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>74.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="94736768"/>
+        <c:axId val="94757248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94736768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>DB</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" baseline="0"/>
+                  <a:t> Threshold</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94757248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94757248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>Avg. Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94736768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>thresholds!$G$34:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.0909090909090905E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5454545454545452E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2727272727272726E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>thresholds!$F$34:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.3146199814830402E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7565019779479841E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8196279774429763E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9248379766012964E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9458799764329603E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9458799764329603E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9458799764329603E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9458799764329603E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="96187520"/>
+        <c:axId val="94699520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="96187520"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="94699520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94699520"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="96187520"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1375,11 +2651,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="76185984"/>
-        <c:axId val="76187904"/>
+        <c:axId val="62227200"/>
+        <c:axId val="62229120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76185984"/>
+        <c:axId val="62227200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,14 +2681,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76187904"/>
+        <c:crossAx val="62229120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76187904"/>
+        <c:axId val="62229120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +2724,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76185984"/>
+        <c:crossAx val="62227200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,7 +2739,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1574,11 +2850,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="76203136"/>
-        <c:axId val="76205440"/>
+        <c:axId val="62240256"/>
+        <c:axId val="61087744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76203136"/>
+        <c:axId val="62240256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1603,12 +2879,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76205440"/>
+        <c:crossAx val="61087744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76205440"/>
+        <c:axId val="61087744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1651,7 +2927,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76203136"/>
+        <c:crossAx val="62240256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -1664,7 +2940,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1754,11 +3030,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="75557888"/>
-        <c:axId val="76223616"/>
+        <c:axId val="61144448"/>
+        <c:axId val="62592512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75557888"/>
+        <c:axId val="61144448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,16 +3056,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76223616"/>
+        <c:crossAx val="62592512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76223616"/>
+        <c:axId val="62592512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,10 +3088,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75557888"/>
+        <c:crossAx val="61144448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1823,7 +3101,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1913,11 +3191,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76247808"/>
-        <c:axId val="76249728"/>
+        <c:axId val="62612608"/>
+        <c:axId val="62614528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76247808"/>
+        <c:axId val="62612608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,16 +3217,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76249728"/>
+        <c:crossAx val="62614528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76249728"/>
+        <c:axId val="62614528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,10 +3249,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76247808"/>
+        <c:crossAx val="62612608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1982,7 +3262,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2072,11 +3352,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76380416"/>
-        <c:axId val="76394880"/>
+        <c:axId val="63994496"/>
+        <c:axId val="64008960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76380416"/>
+        <c:axId val="63994496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,16 +3378,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76394880"/>
+        <c:crossAx val="64008960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76394880"/>
+        <c:axId val="64008960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,10 +3410,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76380416"/>
+        <c:crossAx val="63994496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2141,7 +3423,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2195,22 +3477,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76308480"/>
-        <c:axId val="76310016"/>
+        <c:axId val="64250240"/>
+        <c:axId val="64251776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76308480"/>
+        <c:axId val="64250240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76310016"/>
+        <c:crossAx val="64251776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76310016"/>
+        <c:axId val="64251776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,19 +3500,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76308480"/>
+        <c:crossAx val="64250240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2493,11 +3776,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="76589696"/>
-        <c:axId val="76448512"/>
+        <c:axId val="66366464"/>
+        <c:axId val="63857792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76589696"/>
+        <c:axId val="66366464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2520,15 +3803,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76448512"/>
+        <c:crossAx val="63857792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76448512"/>
+        <c:axId val="63857792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2551,16 +3835,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76589696"/>
+        <c:crossAx val="66366464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2572,7 +3858,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2599,6 +3885,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -2654,6 +3941,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>14</c:v>
                 </c:pt>
@@ -2919,11 +4209,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76471296"/>
-        <c:axId val="76608640"/>
+        <c:axId val="63888768"/>
+        <c:axId val="66373120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76471296"/>
+        <c:axId val="63888768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2945,17 +4235,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76608640"/>
+        <c:crossAx val="66373120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76608640"/>
+        <c:axId val="66373120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,22 +4269,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76471296"/>
+        <c:crossAx val="63888768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3279,15 +4572,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3338,16 +4631,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3361,6 +4654,131 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="グラフ 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="グラフ 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="グラフ 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3982,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3992,7 +5410,7 @@
     <col min="2" max="3" width="9" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="1.625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="9" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="1.75" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
   </cols>
@@ -4461,6 +5879,629 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12">
+        <v>102.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="12">
+        <v>102.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12">
+        <v>102.27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12">
+        <v>103.05</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12">
+        <v>103.49</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>102.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>0.9</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>0.8</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>0.7</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>0.5</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>0.3</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B34">
+        <v>110</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>118</v>
+      </c>
+      <c r="F34">
+        <f>(B34/B45)</f>
+        <v>2.3146199814830402E-3</v>
+      </c>
+      <c r="G34">
+        <f>(C34/B44)</f>
+        <v>9.0909090909090905E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>131</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>120</v>
+      </c>
+      <c r="F35">
+        <f>(B35/B45)</f>
+        <v>2.7565019779479841E-3</v>
+      </c>
+      <c r="G35">
+        <f>(C35/B44)</f>
+        <v>4.5454545454545452E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>0.9</v>
+      </c>
+      <c r="B36">
+        <v>134</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>117</v>
+      </c>
+      <c r="F36">
+        <f>(B36/B45)</f>
+        <v>2.8196279774429763E-3</v>
+      </c>
+      <c r="G36">
+        <f>(C36/B44)</f>
+        <v>2.2727272727272726E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>0.8</v>
+      </c>
+      <c r="B37">
+        <v>139</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>117</v>
+      </c>
+      <c r="F37">
+        <f>(B37/B45)</f>
+        <v>2.9248379766012964E-3</v>
+      </c>
+      <c r="G37">
+        <f>(C37/B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>0.7</v>
+      </c>
+      <c r="B38">
+        <v>140</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>118</v>
+      </c>
+      <c r="F38">
+        <f>(B38/B45)</f>
+        <v>2.9458799764329603E-3</v>
+      </c>
+      <c r="G38">
+        <f>(C38/B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>0.5</v>
+      </c>
+      <c r="B39">
+        <v>140</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>120</v>
+      </c>
+      <c r="F39">
+        <f>(B39/B45)</f>
+        <v>2.9458799764329603E-3</v>
+      </c>
+      <c r="G39">
+        <f>(C39/B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>0.3</v>
+      </c>
+      <c r="B40">
+        <v>140</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>121</v>
+      </c>
+      <c r="F40">
+        <f>(B40/B45)</f>
+        <v>2.9458799764329603E-3</v>
+      </c>
+      <c r="G40">
+        <f>(C40/B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>0.1</v>
+      </c>
+      <c r="B41">
+        <v>140</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>120</v>
+      </c>
+      <c r="F41">
+        <f>(B41/B45)</f>
+        <v>2.9458799764329603E-3</v>
+      </c>
+      <c r="G41">
+        <f>(C41/B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45">
+        <v>47524</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6593,7 +8634,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6788,7 +8829,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>14</v>
@@ -6933,7 +8974,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="2">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -7700,8 +9741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7909,6 +9950,9 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
       <c r="C10" s="2">
         <v>14</v>
       </c>
@@ -8067,6 +10111,9 @@
     <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>28</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Scripts for running tests, in order to make RoC graph. For both CGO and SUJ algorithm.
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="suj" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="all" sheetId="9" r:id="rId9"/>
     <sheet name="robust" sheetId="10" r:id="rId10"/>
     <sheet name="thresholds" sheetId="11" r:id="rId11"/>
+    <sheet name="cgo thresholds" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="96">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -347,12 +348,80 @@
     <t>FNR</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>L3 (multi)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L2 (multi)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>l2fact</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.1 _ 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.06 _ 5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.03 _ 10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 _ 15</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.96 _ 20</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.93 _ 25</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.9 _ 30</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.86 _ 35</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.83 _ 40</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.8 _ 45</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.76 _ 50</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L3 _ L2 (multi)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>l3 _ l2 thresh</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +458,14 @@
       <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -453,7 +530,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -501,6 +578,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2384,7 +2479,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2468,12 +2563,11 @@
                   <c:v>2.9458799764329603E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9458799764329603E-3</c:v>
+                  <c:v>2.651291978789664E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
         </c:ser>
         <c:axId val="96187520"/>
         <c:axId val="94699520"/>
@@ -2539,7 +2633,948 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>thresholds!$G$50:$G$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>thresholds!$F$50:$F$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7855399377156805E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1236427910108577E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0442723676458209E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0490699436074403E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9765171281878636E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.9765171281878636E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9765171281878636E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9765171281878636E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9765171281878636E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="92918528"/>
+        <c:axId val="100508032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="92918528"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0000000000000004E-7"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="100508032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="100508032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0000000000000004E-6"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="92918528"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$G$34:$G$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73333333333333328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$F$34:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5319616596043596E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1723731617230517E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3142688812852642E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8068477940676623E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6136955881353247E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4456957694137908E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9804672452471053E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.556026376016859E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0454782352541299E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.362715551426435E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5485259794702136E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6210373660238836E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7207405225351793E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7615281774716187E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7977838707484533E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8385715256848926E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8702952573021233E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8929550656001451E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9020189889193537E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:alpha val="0"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>thresholds!$G$67:$G$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>thresholds!$F$67:$F$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3863477629600016E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3863477629600017E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9001837941553338E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7494965261049344E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8520980722261355E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="359084800"/>
+        <c:axId val="359086336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="359084800"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0000000000000002E-3"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="359086336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="359086336"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="359084800"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>thresholds!$G$85:$G$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>thresholds!$F$85:$F$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6.312599949499201E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7855399377156805E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6602979547176165E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.336166989310664E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9884689840922481E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6365625789074993E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9627135762982915E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.013214375894285E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3309485733524116E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9858597761131218E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7985859776113124E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="102722176"/>
+        <c:axId val="141945088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="102722176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0000000000000013E-7"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="141945088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="141945088"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0000000000000012E-6"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="102722176"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$G$34:$G$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73333333333333328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$F$34:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5319616596043596E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1723731617230517E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3142688812852642E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8068477940676623E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6136955881353247E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4456957694137908E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9804672452471053E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.556026376016859E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0454782352541299E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.362715551426435E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5485259794702136E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6210373660238836E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7207405225351793E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7615281774716187E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7977838707484533E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8385715256848926E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8702952573021233E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8929550656001451E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9020189889193537E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="209995264"/>
+        <c:axId val="209997184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="209995264"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="209997184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="209997184"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="209995264"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4306,6 +5341,41 @@
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4784,6 +5854,96 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5884,18 +7044,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:X111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="M55" workbookViewId="0">
+      <selection activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="22" max="22" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6463,7 +7625,7 @@
         <v>0.1</v>
       </c>
       <c r="B41">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -6473,7 +7635,7 @@
       </c>
       <c r="F41">
         <f>(B41/B45)</f>
-        <v>2.9458799764329603E-3</v>
+        <v>2.651291978789664E-3</v>
       </c>
       <c r="G41">
         <f>(C41/B44)</f>
@@ -6493,6 +7655,2143 @@
         <v>77</v>
       </c>
       <c r="B45">
+        <v>47524</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>25</v>
+      </c>
+      <c r="D50">
+        <v>118</v>
+      </c>
+      <c r="F50">
+        <f>(B50/(B63))</f>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f>(C50/B62)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>37</v>
+      </c>
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <v>120</v>
+      </c>
+      <c r="F51">
+        <f>(B51/(B63))</f>
+        <v>7.7855399377156805E-4</v>
+      </c>
+      <c r="G51">
+        <f>(C51/B62)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>0.9</v>
+      </c>
+      <c r="B52">
+        <v>534</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>117</v>
+      </c>
+      <c r="F52">
+        <f>(B52/(B63))</f>
+        <v>1.1236427910108577E-2</v>
+      </c>
+      <c r="G52">
+        <f>(C52/B62)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>0.8</v>
+      </c>
+      <c r="B53">
+        <v>1922</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>117</v>
+      </c>
+      <c r="F53">
+        <f>(B53/(B63))</f>
+        <v>4.0442723676458209E-2</v>
+      </c>
+      <c r="G53">
+        <f>(C53/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>0.7</v>
+      </c>
+      <c r="B54">
+        <v>3350</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>118</v>
+      </c>
+      <c r="F54">
+        <f>(B54/(B63))</f>
+        <v>7.0490699436074403E-2</v>
+      </c>
+      <c r="G54">
+        <f>(C54/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>0.6</v>
+      </c>
+      <c r="B55">
+        <v>4266</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f>(B55/(B63))</f>
+        <v>8.9765171281878636E-2</v>
+      </c>
+      <c r="G55">
+        <f>(C55/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>0.5</v>
+      </c>
+      <c r="B56">
+        <v>4266</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>120</v>
+      </c>
+      <c r="F56">
+        <f>(B56/(B63))</f>
+        <v>8.9765171281878636E-2</v>
+      </c>
+      <c r="G56">
+        <f>(C56/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>0.3</v>
+      </c>
+      <c r="B57">
+        <v>4266</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>121</v>
+      </c>
+      <c r="F57">
+        <f>(B57/(B63))</f>
+        <v>8.9765171281878636E-2</v>
+      </c>
+      <c r="G57">
+        <f>(C57/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58">
+        <v>0.1</v>
+      </c>
+      <c r="B58">
+        <v>4266</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>120</v>
+      </c>
+      <c r="F58">
+        <f>(B58/(B63))</f>
+        <v>8.9765171281878636E-2</v>
+      </c>
+      <c r="G58">
+        <f>(C58/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>0.1</v>
+      </c>
+      <c r="B59">
+        <v>4266</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>120</v>
+      </c>
+      <c r="F59">
+        <f>(B59/(B63))</f>
+        <v>8.9765171281878636E-2</v>
+      </c>
+      <c r="G59">
+        <f>(C59/B62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63">
+        <v>47524</v>
+      </c>
+      <c r="C63">
+        <v>24506406</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24">
+      <c r="A65" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" t="s">
+        <v>73</v>
+      </c>
+      <c r="R65" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X65" s="3"/>
+    </row>
+    <row r="66" spans="1:24">
+      <c r="A66" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T66" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>25</v>
+      </c>
+      <c r="D67">
+        <v>118</v>
+      </c>
+      <c r="F67">
+        <f>(B67/(B80))</f>
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <f>(C67/B79)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="Q67">
+        <v>1.2</v>
+      </c>
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="W67">
+        <f>(S67/(S67+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X67">
+        <f>(S81/(S81+S67))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>11</v>
+      </c>
+      <c r="D68">
+        <v>120</v>
+      </c>
+      <c r="F68">
+        <f>(B68/(B80))</f>
+        <v>5.3863477629600016E-6</v>
+      </c>
+      <c r="G68">
+        <f>(C68/B79)</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="Q68">
+        <v>1.175</v>
+      </c>
+      <c r="R68">
+        <v>5</v>
+      </c>
+      <c r="W68">
+        <f>(S68/(S68+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X68">
+        <f>(S81/(S81+S68))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24">
+      <c r="A69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69">
+        <v>180</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>117</v>
+      </c>
+      <c r="F69">
+        <f>(B69/(B80))</f>
+        <v>5.3863477629600017E-5</v>
+      </c>
+      <c r="G69">
+        <f>(C69/B79)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Q69">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R69">
+        <v>10</v>
+      </c>
+      <c r="W69">
+        <f>(S69/(S69+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X69">
+        <f>(S81/(S81+S69))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24">
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70">
+        <v>635</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>117</v>
+      </c>
+      <c r="F70">
+        <f>(B70/(B80))</f>
+        <v>1.9001837941553338E-4</v>
+      </c>
+      <c r="G70">
+        <f>(C70/B79)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="Q70">
+        <v>1.125</v>
+      </c>
+      <c r="R70">
+        <v>15</v>
+      </c>
+      <c r="W70">
+        <f>(S70/(S70+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X70">
+        <f>(S81/(S81+S70))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24">
+      <c r="A71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71">
+        <v>1253</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>118</v>
+      </c>
+      <c r="F71">
+        <f>(B71/(B80))</f>
+        <v>3.7494965261049344E-4</v>
+      </c>
+      <c r="G71">
+        <f>(C71/B79)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q71">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R71">
+        <v>20</v>
+      </c>
+      <c r="W71">
+        <f>(S71/(S71+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <f>(S81/(S81+S71))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="13.5" hidden="1" customHeight="1">
+      <c r="A72" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72">
+        <v>2000</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <f>(B72/(B80))</f>
+        <v>5.9848308477333356E-4</v>
+      </c>
+      <c r="G72">
+        <f>(C72/B79)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="R72" t="s">
+        <v>88</v>
+      </c>
+      <c r="W72">
+        <f>(S72/(S72+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X72">
+        <f>(S81/(S81+S72))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" ht="13.5" hidden="1" customHeight="1">
+      <c r="A73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73">
+        <v>2416</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>120</v>
+      </c>
+      <c r="F73">
+        <f>(B73/(B80))</f>
+        <v>7.2296756640618685E-4</v>
+      </c>
+      <c r="G73">
+        <f>(C73/B79)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="R73" t="s">
+        <v>89</v>
+      </c>
+      <c r="W73">
+        <f>(S73/(S73+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X73">
+        <f>(S81/(S81+S73))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24">
+      <c r="A74" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74">
+        <v>2624</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>121</v>
+      </c>
+      <c r="F74">
+        <f>(B74/(B80))</f>
+        <v>7.8520980722261355E-4</v>
+      </c>
+      <c r="G74">
+        <f>(C74/B79)</f>
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>1.075</v>
+      </c>
+      <c r="R74">
+        <v>25</v>
+      </c>
+      <c r="W74">
+        <f>(S74/(S74+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X74">
+        <f>(S81/(S81+S74))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75">
+        <v>3399</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>120</v>
+      </c>
+      <c r="F75">
+        <f>(B75/(B80))</f>
+        <v>1.0171220025722804E-3</v>
+      </c>
+      <c r="G75">
+        <f>(C75/B79)</f>
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>1.05</v>
+      </c>
+      <c r="R75">
+        <v>30</v>
+      </c>
+      <c r="W75">
+        <f>(S75/(S75+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X75">
+        <f>(S81/(S81+S75))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76">
+        <v>3399</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>120</v>
+      </c>
+      <c r="F76">
+        <f>(B76/(B80))</f>
+        <v>1.0171220025722804E-3</v>
+      </c>
+      <c r="G76">
+        <f>(C76/B79)</f>
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="R76">
+        <v>35</v>
+      </c>
+      <c r="W76">
+        <f>(S76/(S76+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X76">
+        <f>(S81/(S81+S76))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24">
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77">
+        <v>3399</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f>(B77/(B80))</f>
+        <v>1.0171220025722804E-3</v>
+      </c>
+      <c r="G77">
+        <f>(C77/B79)</f>
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+      <c r="R77">
+        <v>40</v>
+      </c>
+      <c r="W77">
+        <f>(S79/(S79+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X77">
+        <f>(S81/(S81+S79))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24">
+      <c r="Q78">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R78">
+        <v>45</v>
+      </c>
+      <c r="W78">
+        <f>(S79/(S79+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X78">
+        <f>(S81/(S81+S79))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24">
+      <c r="A79" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="Q79">
+        <v>0.95</v>
+      </c>
+      <c r="R79">
+        <v>50</v>
+      </c>
+      <c r="W79">
+        <f>(S79/(S79+S82))</f>
+        <v>0</v>
+      </c>
+      <c r="X79">
+        <f>(S81/(S81+S79))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24">
+      <c r="A80" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>3341782</v>
+      </c>
+      <c r="C80">
+        <v>3341782</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
+      <c r="C81">
+        <v>47524</v>
+      </c>
+      <c r="R81" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S81">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
+      <c r="R82" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S82">
+        <v>3341782</v>
+      </c>
+      <c r="T82">
+        <v>24506406</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
+      <c r="A83" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
+      <c r="A84" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <v>24</v>
+      </c>
+      <c r="D85">
+        <v>118</v>
+      </c>
+      <c r="F85">
+        <f>(B85/(B98))</f>
+        <v>6.312599949499201E-5</v>
+      </c>
+      <c r="G85">
+        <f>(C85/B97)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
+      <c r="A86">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>37</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <v>120</v>
+      </c>
+      <c r="F86">
+        <f>(B86/(B98))</f>
+        <v>7.7855399377156805E-4</v>
+      </c>
+      <c r="G86">
+        <f>(C86/B97)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87">
+        <v>269</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>117</v>
+      </c>
+      <c r="F87">
+        <f>(B87/(B98))</f>
+        <v>5.6602979547176165E-3</v>
+      </c>
+      <c r="G87">
+        <f>(C87/B97)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
+      <c r="A88">
+        <v>15</v>
+      </c>
+      <c r="B88">
+        <v>635</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>117</v>
+      </c>
+      <c r="F88">
+        <f>(B88/(B98))</f>
+        <v>1.336166989310664E-2</v>
+      </c>
+      <c r="G88">
+        <f>(C88/B97)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
+      <c r="A89">
+        <v>20</v>
+      </c>
+      <c r="B89">
+        <v>945</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>118</v>
+      </c>
+      <c r="F89">
+        <f>(B89/(B98))</f>
+        <v>1.9884689840922481E-2</v>
+      </c>
+      <c r="G89">
+        <f>(C89/B97)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
+      <c r="A90">
+        <v>25</v>
+      </c>
+      <c r="B90">
+        <v>1253</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="F90">
+        <f>(B90/(B98))</f>
+        <v>2.6365625789074993E-2</v>
+      </c>
+      <c r="G90">
+        <f>(C90/B97)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
+      <c r="A91">
+        <v>30</v>
+      </c>
+      <c r="B91">
+        <v>1408</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>120</v>
+      </c>
+      <c r="F91">
+        <f>(B91/(B98))</f>
+        <v>2.9627135762982915E-2</v>
+      </c>
+      <c r="G91">
+        <f>(C91/B97)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
+      <c r="A92">
+        <v>35</v>
+      </c>
+      <c r="B92">
+        <v>1432</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>121</v>
+      </c>
+      <c r="F92">
+        <f>(B92/(B98))</f>
+        <v>3.013214375894285E-2</v>
+      </c>
+      <c r="G92">
+        <f>(C92/B97)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
+      <c r="A93">
+        <v>40</v>
+      </c>
+      <c r="B93">
+        <v>1583</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>120</v>
+      </c>
+      <c r="F93">
+        <f>(B93/(B98))</f>
+        <v>3.3309485733524116E-2</v>
+      </c>
+      <c r="G93">
+        <f>(C93/B97)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
+      <c r="A94">
+        <v>45</v>
+      </c>
+      <c r="B94">
+        <v>1419</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>120</v>
+      </c>
+      <c r="F94">
+        <f>(B94/(B98))</f>
+        <v>2.9858597761131218E-2</v>
+      </c>
+      <c r="G94">
+        <f>(C94/B97)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
+      <c r="A95">
+        <v>50</v>
+      </c>
+      <c r="B95">
+        <v>1330</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <f>(B95/(B98))</f>
+        <v>2.7985859776113124E-2</v>
+      </c>
+      <c r="G95">
+        <f>(C95/B97)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B98">
+        <v>47524</v>
+      </c>
+      <c r="C98">
+        <v>3341782</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="16"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="16"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="16"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="16"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="16"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="8"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="16"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="16"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="16"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="8"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="16"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="8"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="8"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+      <c r="I109" s="8"/>
+      <c r="J109" s="8"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
+      <c r="J110" s="8"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="8"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="22" max="22" width="3.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12">
+        <v>102.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="12">
+        <v>102.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12">
+        <v>102.27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12">
+        <v>103.05</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12">
+        <v>103.49</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>102.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>0.9</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>0.8</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>0.7</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>0.5</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>0.3</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="19">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>118</v>
+      </c>
+      <c r="F34">
+        <f>(B34/B57)</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>(C34/B56)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>120</v>
+      </c>
+      <c r="F35">
+        <f>(B35/B57)</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>(C35/B56)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>117</v>
+      </c>
+      <c r="F36">
+        <f>(B36/B57)</f>
+        <v>4.5319616596043596E-6</v>
+      </c>
+      <c r="G36">
+        <f>(C36/B56)</f>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>27</v>
+      </c>
+      <c r="D37">
+        <v>117</v>
+      </c>
+      <c r="F37">
+        <f>(B37/B57)</f>
+        <v>3.1723731617230517E-5</v>
+      </c>
+      <c r="G37">
+        <f>(C37/B56)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="B38">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>27</v>
+      </c>
+      <c r="D38">
+        <v>118</v>
+      </c>
+      <c r="F38">
+        <f>(B38/B57)</f>
+        <v>1.3142688812852642E-4</v>
+      </c>
+      <c r="G38">
+        <f>(C38/B56)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="B39">
+        <v>84</v>
+      </c>
+      <c r="C39">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>120</v>
+      </c>
+      <c r="F39">
+        <f>(B39/B57)</f>
+        <v>3.8068477940676623E-4</v>
+      </c>
+      <c r="G39">
+        <f>(C39/B56)</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="B40">
+        <v>168</v>
+      </c>
+      <c r="C40">
+        <v>22</v>
+      </c>
+      <c r="D40">
+        <v>121</v>
+      </c>
+      <c r="F40">
+        <f>(B40/B57)</f>
+        <v>7.6136955881353247E-4</v>
+      </c>
+      <c r="G40">
+        <f>(C40/B56)</f>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="B41">
+        <v>319</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41">
+        <v>120</v>
+      </c>
+      <c r="F41">
+        <f>(B41/B57)</f>
+        <v>1.4456957694137908E-3</v>
+      </c>
+      <c r="G41">
+        <f>(C41/B56)</f>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="B42">
+        <v>437</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <f>(B42/B57)</f>
+        <v>1.9804672452471053E-3</v>
+      </c>
+      <c r="G42">
+        <f>(C42/B56)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="B43">
+        <v>564</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <f>(B43/B57)</f>
+        <v>2.556026376016859E-3</v>
+      </c>
+      <c r="G43">
+        <f>(C43/B56)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="B44">
+        <v>672</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <f>(B44/B57)</f>
+        <v>3.0454782352541299E-3</v>
+      </c>
+      <c r="G44">
+        <f>(C44/B56)</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B45" s="8">
+        <v>742</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <f>(B45/B57)</f>
+        <v>3.362715551426435E-3</v>
+      </c>
+      <c r="G45">
+        <f>(C45/B56)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="B46" s="4">
+        <v>783</v>
+      </c>
+      <c r="C46" s="8">
+        <v>2</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46">
+        <f>(B46/B57)</f>
+        <v>3.5485259794702136E-3</v>
+      </c>
+      <c r="G46">
+        <f>(C46/B56)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="20">
+        <v>0.65</v>
+      </c>
+      <c r="B47" s="4">
+        <v>799</v>
+      </c>
+      <c r="C47" s="4">
+        <v>2</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47">
+        <f>(B47/B57)</f>
+        <v>3.6210373660238836E-3</v>
+      </c>
+      <c r="G47">
+        <f>(C47/B56)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="B48" s="4">
+        <v>821</v>
+      </c>
+      <c r="C48" s="4">
+        <v>2</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48">
+        <f>(B48/B57)</f>
+        <v>3.7207405225351793E-3</v>
+      </c>
+      <c r="G48">
+        <f>(C48/B56)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="B49" s="4">
+        <v>830</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49">
+        <f>(B49/B57)</f>
+        <v>3.7615281774716187E-3</v>
+      </c>
+      <c r="G49">
+        <f>(C49/B56)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="B50" s="4">
+        <v>838</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <f>(B50/B57)</f>
+        <v>3.7977838707484533E-3</v>
+      </c>
+      <c r="G50">
+        <f>(C50/B56)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="21">
+        <v>0.85</v>
+      </c>
+      <c r="B51" s="4">
+        <v>847</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f>(B51/B57)</f>
+        <v>3.8385715256848926E-3</v>
+      </c>
+      <c r="G51">
+        <f>(C51/B56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="B52" s="4">
+        <v>854</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52">
+        <f>(B52/B57)</f>
+        <v>3.8702952573021233E-3</v>
+      </c>
+      <c r="G52">
+        <f>(C52/B56)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="B53" s="4">
+        <v>859</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>(B53/B57)</f>
+        <v>3.8929550656001451E-3</v>
+      </c>
+      <c r="G53">
+        <f>(C53/B56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="21">
+        <v>1</v>
+      </c>
+      <c r="B54" s="4">
+        <v>861</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <f>(B54/B57)</f>
+        <v>3.9020189889193537E-3</v>
+      </c>
+      <c r="G54">
+        <f>(C54/B56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57">
+        <v>220655</v>
+      </c>
+      <c r="C57">
+        <v>220655</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="C58">
         <v>47524</v>
       </c>
     </row>
@@ -9741,8 +13040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" activeCellId="1" sqref="E19 E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
Latest results for the ISCIT 2010 conference paper.
</commit_message>
<xml_diff>
--- a/documents/vfp_paper_results.xlsx
+++ b/documents/vfp_paper_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="7440" windowHeight="4875" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="6690" windowHeight="4725" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="suj" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="96">
   <si>
     <t>Avg. run-times</t>
     <phoneticPr fontId="1"/>
@@ -418,8 +418,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -579,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -588,13 +588,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -697,11 +697,11 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:axId val="61057280"/>
-        <c:axId val="61076224"/>
+        <c:axId val="72104576"/>
+        <c:axId val="72131712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61057280"/>
+        <c:axId val="72104576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,14 +725,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61076224"/>
+        <c:crossAx val="72131712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61076224"/>
+        <c:axId val="72131712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +758,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61057280"/>
+        <c:crossAx val="72104576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -767,7 +767,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1130,11 +1130,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="66449408"/>
-        <c:axId val="66451328"/>
+        <c:axId val="89403776"/>
+        <c:axId val="89405696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66449408"/>
+        <c:axId val="89403776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1161,16 +1161,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66451328"/>
+        <c:crossAx val="89405696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66451328"/>
+        <c:axId val="89405696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,24 +1192,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66449408"/>
+        <c:crossAx val="89403776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1237,7 +1234,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1561,11 +1557,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="66490368"/>
-        <c:axId val="66492288"/>
+        <c:axId val="89440640"/>
+        <c:axId val="89442560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66490368"/>
+        <c:axId val="89440640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,18 +1587,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66492288"/>
+        <c:crossAx val="89442560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66492288"/>
+        <c:axId val="89442560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,24 +1620,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66490368"/>
+        <c:crossAx val="89440640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1669,7 +1662,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1835,11 +1827,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="42851328"/>
-        <c:axId val="42861696"/>
+        <c:axId val="84093952"/>
+        <c:axId val="84116608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42851328"/>
+        <c:axId val="84093952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,18 +1857,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42861696"/>
+        <c:crossAx val="84116608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42861696"/>
+        <c:axId val="84116608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,24 +1890,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42851328"/>
+        <c:crossAx val="84093952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1943,7 +1932,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -2109,11 +2097,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78793344"/>
-        <c:axId val="81773312"/>
+        <c:axId val="84133760"/>
+        <c:axId val="89456640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78793344"/>
+        <c:axId val="84133760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,18 +2123,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81773312"/>
+        <c:crossAx val="89456640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81773312"/>
+        <c:axId val="89456640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2169,24 +2156,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78793344"/>
+        <c:crossAx val="84133760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2386,11 +2371,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94736768"/>
-        <c:axId val="94757248"/>
+        <c:axId val="89506560"/>
+        <c:axId val="89508480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94736768"/>
+        <c:axId val="89506560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -2417,16 +2402,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94757248"/>
+        <c:crossAx val="89508480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94757248"/>
+        <c:axId val="89508480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,24 +2433,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94736768"/>
+        <c:crossAx val="89506560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2569,11 +2551,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="96187520"/>
-        <c:axId val="94699520"/>
+        <c:axId val="89655552"/>
+        <c:axId val="89706880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96187520"/>
+        <c:axId val="89655552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2595,12 +2577,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94699520"/>
+        <c:crossAx val="89706880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94699520"/>
+        <c:axId val="89706880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2614,7 +2596,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="96187520"/>
+        <c:crossAx val="89655552"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2633,7 +2615,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2748,15 +2730,15 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92918528"/>
-        <c:axId val="100508032"/>
+        <c:axId val="89713280"/>
+        <c:axId val="89731840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92918528"/>
+        <c:axId val="89713280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000004E-7"/>
+          <c:min val="1.0000000000000013E-7"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
@@ -2775,16 +2757,16 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="100508032"/>
+        <c:crossAx val="89731840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100508032"/>
+        <c:axId val="89731840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000004E-6"/>
+          <c:min val="1.0000000000000012E-6"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:majorGridlines/>
@@ -2795,7 +2777,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="92918528"/>
+        <c:crossAx val="89713280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2814,7 +2796,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2825,12 +2807,25 @@
   <c:lang val="ja-JP"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18938240859427455"/>
+          <c:y val="0.1012111255877188"/>
+          <c:w val="0.71801306232069828"/>
+          <c:h val="0.68446798466738423"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>CGO</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="12700">
               <a:solidFill>
@@ -2998,6 +2993,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>SUJ</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="15875">
               <a:solidFill>
@@ -3026,7 +3024,7 @@
               <c:f>thresholds!$G$67:$G$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.83333333333333337</c:v>
                 </c:pt>
@@ -3034,15 +3032,21 @@
                   <c:v>0.36666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6.6666666666666666E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>3.3333333333333333E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3053,7 +3057,7 @@
               <c:f>thresholds!$F$67:$F$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3061,7 +3065,7 @@
                   <c:v>5.3863477629600016E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3863477629600017E-5</c:v>
+                  <c:v>9.3363361224640024E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.9001837941553338E-4</c:v>
@@ -3070,24 +3074,60 @@
                   <c:v>3.7494965261049344E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>5.9848308477333356E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.2296756640618685E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.8520980722261355E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="359084800"/>
-        <c:axId val="359086336"/>
+        <c:axId val="89764608"/>
+        <c:axId val="89766528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359084800"/>
+        <c:axId val="89764608"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000002E-3"/>
+          <c:min val="1.0000000000000007E-3"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>P</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" sz="600"/>
+                  <a:t>FA</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.91472990294817802"/>
+              <c:y val="0.74961611812911877"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -3103,18 +3143,49 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="359086336"/>
+        <c:crossAx val="89766528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359086336"/>
+        <c:axId val="89766528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>P</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP" sz="600"/>
+                  <a:t>FR</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.19212403100775188"/>
+              <c:y val="2.378066051096131E-2"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="in"/>
@@ -3122,7 +3193,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="359084800"/>
+        <c:crossAx val="89764608"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3137,11 +3208,20 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3262,15 +3342,15 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102722176"/>
-        <c:axId val="141945088"/>
+        <c:axId val="89780608"/>
+        <c:axId val="89782528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102722176"/>
+        <c:axId val="89780608"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000013E-7"/>
+          <c:min val="1.0000000000000022E-7"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
@@ -3289,16 +3369,16 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141945088"/>
+        <c:crossAx val="89782528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141945088"/>
+        <c:axId val="89782528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000012E-6"/>
+          <c:min val="1.0000000000000021E-6"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:majorGridlines/>
@@ -3309,7 +3389,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="102722176"/>
+        <c:crossAx val="89780608"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3328,7 +3408,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3366,10 +3446,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'cgo thresholds'!$G$34:$G$54</c:f>
+              <c:f>thresholds!$X$85:$X$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3377,71 +3457,41 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96666666666666667</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>7.7720207253886009E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73333333333333328</c:v>
+                  <c:v>4.1039671682626538E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56666666666666665</c:v>
+                  <c:v>2.5125628140703519E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>1.3774104683195593E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2</c:v>
+                  <c:v>1.3774104683195593E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.6666666666666666E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.6666666666666666E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.6666666666666666E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.3333333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.3333333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1.3774104683195593E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'cgo thresholds'!$F$34:$F$54</c:f>
+              <c:f>thresholds!$W$85:$W$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3449,74 +3499,45 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5319616596043596E-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1723731617230517E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3142688812852642E-4</c:v>
+                  <c:v>1.6158782178419287E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8068477940676623E-4</c:v>
+                  <c:v>1.0651864165991949E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.6136955881353247E-4</c:v>
+                  <c:v>2.0972432769291572E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4456957694137908E-3</c:v>
+                  <c:v>3.4819587274218607E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9804672452471053E-3</c:v>
+                  <c:v>6.4235794409571965E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.556026376016859E-3</c:v>
+                  <c:v>6.4235794409571965E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0454782352541299E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.362715551426435E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.5485259794702136E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.6210373660238836E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.7207405225351793E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.7615281774716187E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.7977838707484533E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.8385715256848926E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.8702952573021233E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.8929550656001451E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.9020189889193537E-3</c:v>
+                  <c:v>6.4235794409571965E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="209995264"/>
-        <c:axId val="209997184"/>
+        <c:axId val="89629440"/>
+        <c:axId val="89631360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209995264"/>
+        <c:axId val="89629440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="1.000000000000003E-7"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
@@ -3535,16 +3556,16 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209997184"/>
+        <c:crossAx val="89631360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209997184"/>
+        <c:axId val="89631360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:min val="1.0000000000000025E-6"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:majorGridlines/>
@@ -3555,7 +3576,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="209995264"/>
+        <c:crossAx val="89629440"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3574,7 +3595,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3686,11 +3707,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="62227200"/>
-        <c:axId val="62229120"/>
+        <c:axId val="72512640"/>
+        <c:axId val="72514560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62227200"/>
+        <c:axId val="72512640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,14 +3737,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62229120"/>
+        <c:crossAx val="72514560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62229120"/>
+        <c:axId val="72514560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3759,7 +3780,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62227200"/>
+        <c:crossAx val="72512640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3774,7 +3795,253 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ja-JP"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$G$34:$G$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73333333333333328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cgo thresholds'!$F$34:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5319616596043596E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1723731617230517E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3142688812852642E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8068477940676623E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6136955881353247E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4456957694137908E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9804672452471053E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.556026376016859E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0454782352541299E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.362715551426435E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5485259794702136E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6210373660238836E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7207405225351793E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7615281774716187E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7977838707484533E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8385715256848926E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8702952573021233E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8929550656001451E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9020189889193537E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="89762048"/>
+        <c:axId val="89792896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="89762048"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln cap="flat">
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="50000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="89792896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="89792896"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="89762048"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF">
+              <a:lumMod val="50000"/>
+            </a:sysClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3885,11 +4152,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="62240256"/>
-        <c:axId val="61087744"/>
+        <c:axId val="72505216"/>
+        <c:axId val="83636608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62240256"/>
+        <c:axId val="72505216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -3914,12 +4181,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61087744"/>
+        <c:crossAx val="83636608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61087744"/>
+        <c:axId val="83636608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -3962,7 +4229,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62240256"/>
+        <c:crossAx val="72505216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -3975,7 +4242,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4065,11 +4332,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="61144448"/>
-        <c:axId val="62592512"/>
+        <c:axId val="83701760"/>
+        <c:axId val="83703680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61144448"/>
+        <c:axId val="83701760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4091,17 +4358,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62592512"/>
+        <c:crossAx val="83703680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62592512"/>
+        <c:axId val="83703680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4123,11 +4389,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61144448"/>
+        <c:crossAx val="83701760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4136,7 +4401,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4226,11 +4491,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="62612608"/>
-        <c:axId val="62614528"/>
+        <c:axId val="83768832"/>
+        <c:axId val="83770752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62612608"/>
+        <c:axId val="83768832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4252,17 +4517,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62614528"/>
+        <c:crossAx val="83770752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62614528"/>
+        <c:axId val="83770752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,11 +4548,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62612608"/>
+        <c:crossAx val="83768832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4297,7 +4560,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4387,11 +4650,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="63994496"/>
-        <c:axId val="64008960"/>
+        <c:axId val="83794944"/>
+        <c:axId val="83817600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63994496"/>
+        <c:axId val="83794944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4413,17 +4676,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64008960"/>
+        <c:crossAx val="83817600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64008960"/>
+        <c:axId val="83817600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4445,11 +4707,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63994496"/>
+        <c:crossAx val="83794944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4458,7 +4719,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4512,22 +4773,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64250240"/>
-        <c:axId val="64251776"/>
+        <c:axId val="75162368"/>
+        <c:axId val="75163904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64250240"/>
+        <c:axId val="75162368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64251776"/>
+        <c:crossAx val="75163904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64251776"/>
+        <c:axId val="75163904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4535,20 +4796,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64250240"/>
+        <c:crossAx val="75162368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4811,11 +5071,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="66366464"/>
-        <c:axId val="63857792"/>
+        <c:axId val="83864960"/>
+        <c:axId val="84047360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66366464"/>
+        <c:axId val="83864960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4838,16 +5098,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63857792"/>
+        <c:crossAx val="84047360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63857792"/>
+        <c:axId val="84047360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4870,18 +5129,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66366464"/>
+        <c:crossAx val="83864960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4893,7 +5150,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4920,7 +5177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -5244,11 +5500,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="63888768"/>
-        <c:axId val="66373120"/>
+        <c:axId val="83959808"/>
+        <c:axId val="83961728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63888768"/>
+        <c:axId val="83959808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5270,18 +5526,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66373120"/>
+        <c:crossAx val="83961728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66373120"/>
+        <c:axId val="83961728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5304,24 +5559,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63888768"/>
+        <c:crossAx val="83959808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5889,13 +6142,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5939,6 +6192,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="グラフ 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7046,8 +7329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M55" workbookViewId="0">
-      <selection activeCell="S67" sqref="S67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7928,26 +8211,15 @@
         <v>24506406</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:7">
       <c r="A65" s="17" t="s">
         <v>94</v>
       </c>
       <c r="F65" t="s">
         <v>73</v>
       </c>
-      <c r="R65" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="X65" s="3"/>
-    </row>
-    <row r="66" spans="1:24">
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
         <v>95</v>
       </c>
@@ -7967,25 +8239,8 @@
       <c r="G66" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R66" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="S66" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T66" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="U66" s="3"/>
-      <c r="V66" s="3"/>
-      <c r="W66" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X66" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24">
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -8006,22 +8261,8 @@
         <f>(C67/B79)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q67">
-        <v>1.2</v>
-      </c>
-      <c r="R67">
-        <v>1</v>
-      </c>
-      <c r="W67">
-        <f>(S67/(S67+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X67">
-        <f>(S81/(S81+S67))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24">
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -8042,58 +8283,30 @@
         <f>(C68/B79)</f>
         <v>0.36666666666666664</v>
       </c>
-      <c r="Q68">
-        <v>1.175</v>
-      </c>
-      <c r="R68">
-        <v>5</v>
-      </c>
-      <c r="W68">
-        <f>(S68/(S68+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X68">
-        <f>(S81/(S81+S68))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24">
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>85</v>
       </c>
       <c r="B69">
-        <v>180</v>
+        <v>312</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <v>117</v>
       </c>
       <c r="F69">
         <f>(B69/(B80))</f>
-        <v>5.3863477629600017E-5</v>
+        <v>9.3363361224640024E-5</v>
       </c>
       <c r="G69">
         <f>(C69/B79)</f>
-        <v>0.1</v>
-      </c>
-      <c r="Q69">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R69">
-        <v>10</v>
-      </c>
-      <c r="W69">
-        <f>(S69/(S69+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X69">
-        <f>(S81/(S81+S69))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -8101,7 +8314,7 @@
         <v>635</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D70">
         <v>117</v>
@@ -8112,24 +8325,10 @@
       </c>
       <c r="G70">
         <f>(C70/B79)</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="Q70">
-        <v>1.125</v>
-      </c>
-      <c r="R70">
-        <v>15</v>
-      </c>
-      <c r="W70">
-        <f>(S70/(S70+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X70">
-        <f>(S81/(S81+S70))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24">
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -8137,7 +8336,7 @@
         <v>1253</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D71">
         <v>118</v>
@@ -8148,24 +8347,10 @@
       </c>
       <c r="G71">
         <f>(C71/B79)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="Q71">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="R71">
-        <v>20</v>
-      </c>
-      <c r="W71">
-        <f>(S71/(S71+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X71">
-        <f>(S81/(S81+S71))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" ht="13.5" hidden="1" customHeight="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="13.5" customHeight="1">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -8173,7 +8358,7 @@
         <v>2000</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F72">
         <f>(B72/(B80))</f>
@@ -8181,21 +8366,10 @@
       </c>
       <c r="G72">
         <f>(C72/B79)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="R72" t="s">
-        <v>88</v>
-      </c>
-      <c r="W72">
-        <f>(S72/(S72+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X72">
-        <f>(S81/(S81+S72))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" ht="13.5" hidden="1" customHeight="1">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="13.5" customHeight="1">
       <c r="A73" t="s">
         <v>89</v>
       </c>
@@ -8216,19 +8390,8 @@
         <f>(C73/B79)</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="R73" t="s">
-        <v>89</v>
-      </c>
-      <c r="W73">
-        <f>(S73/(S73+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X73">
-        <f>(S81/(S81+S73))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24">
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -8249,22 +8412,8 @@
         <f>(C74/B79)</f>
         <v>0</v>
       </c>
-      <c r="Q74">
-        <v>1.075</v>
-      </c>
-      <c r="R74">
-        <v>25</v>
-      </c>
-      <c r="W74">
-        <f>(S74/(S74+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X74">
-        <f>(S81/(S81+S74))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24">
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -8285,27 +8434,13 @@
         <f>(C75/B79)</f>
         <v>0</v>
       </c>
-      <c r="Q75">
-        <v>1.05</v>
-      </c>
-      <c r="R75">
-        <v>30</v>
-      </c>
-      <c r="W75">
-        <f>(S75/(S75+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X75">
-        <f>(S81/(S81+S75))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24">
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>92</v>
       </c>
       <c r="B76">
-        <v>3399</v>
+        <v>3993</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -8315,99 +8450,41 @@
       </c>
       <c r="F76">
         <f>(B76/(B80))</f>
-        <v>1.0171220025722804E-3</v>
+        <v>1.1948714787499604E-3</v>
       </c>
       <c r="G76">
         <f>(C76/B79)</f>
         <v>0</v>
       </c>
-      <c r="Q76">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="R76">
-        <v>35</v>
-      </c>
-      <c r="W76">
-        <f>(S76/(S76+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X76">
-        <f>(S81/(S81+S76))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24">
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>93</v>
       </c>
       <c r="B77">
-        <v>3399</v>
+        <v>3783</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="F77">
         <f>(B77/(B80))</f>
-        <v>1.0171220025722804E-3</v>
+        <v>1.1320307548487603E-3</v>
       </c>
       <c r="G77">
         <f>(C77/B79)</f>
         <v>0</v>
       </c>
-      <c r="Q77">
-        <v>1</v>
-      </c>
-      <c r="R77">
-        <v>40</v>
-      </c>
-      <c r="W77">
-        <f>(S79/(S79+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X77">
-        <f>(S81/(S81+S79))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24">
-      <c r="Q78">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="R78">
-        <v>45</v>
-      </c>
-      <c r="W78">
-        <f>(S79/(S79+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X78">
-        <f>(S81/(S81+S79))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24">
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B79">
         <v>30</v>
       </c>
-      <c r="Q79">
-        <v>0.95</v>
-      </c>
-      <c r="R79">
-        <v>50</v>
-      </c>
-      <c r="W79">
-        <f>(S79/(S79+S82))</f>
-        <v>0</v>
-      </c>
-      <c r="X79">
-        <f>(S81/(S81+S79))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:24">
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="3" t="s">
         <v>77</v>
       </c>
@@ -8418,37 +8495,31 @@
         <v>3341782</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:24">
       <c r="C81">
         <v>47524</v>
       </c>
-      <c r="R81" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S81">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20">
-      <c r="R82" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="S82">
-        <v>3341782</v>
-      </c>
-      <c r="T82">
-        <v>24506406</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20">
+    </row>
+    <row r="83" spans="1:24">
       <c r="A83" s="17" t="s">
         <v>81</v>
       </c>
       <c r="F83" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="84" spans="1:20">
+      <c r="R83" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X83" s="3"/>
+    </row>
+    <row r="84" spans="1:24">
       <c r="A84" s="3" t="s">
         <v>82</v>
       </c>
@@ -8468,8 +8539,25 @@
       <c r="G84" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="85" spans="1:20">
+      <c r="R84" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T84" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+      <c r="W84" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24">
       <c r="A85">
         <v>1</v>
       </c>
@@ -8490,8 +8578,28 @@
         <f>(C85/B97)</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="86" spans="1:20">
+      <c r="Q85">
+        <v>1.2</v>
+      </c>
+      <c r="R85">
+        <v>1</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+      <c r="T85">
+        <v>30</v>
+      </c>
+      <c r="W85">
+        <f>(S85/(S85+S98))</f>
+        <v>0</v>
+      </c>
+      <c r="X85">
+        <f>(S97/(S97+S85))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24">
       <c r="A86">
         <v>5</v>
       </c>
@@ -8512,8 +8620,28 @@
         <f>(C86/B97)</f>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="87" spans="1:20">
+      <c r="Q86">
+        <v>1.175</v>
+      </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <v>30</v>
+      </c>
+      <c r="W86">
+        <f>(S86/(S86+S98))</f>
+        <v>0</v>
+      </c>
+      <c r="X86">
+        <f>(S97/(S97+S86))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24">
       <c r="A87">
         <v>10</v>
       </c>
@@ -8534,8 +8662,28 @@
         <f>(C87/B97)</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="88" spans="1:20">
+      <c r="Q87">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R87">
+        <v>10</v>
+      </c>
+      <c r="S87">
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <v>30</v>
+      </c>
+      <c r="W87">
+        <f>(S87/(S87+S98))</f>
+        <v>0</v>
+      </c>
+      <c r="X87">
+        <f>(S97/(S97+S87))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24">
       <c r="A88">
         <v>15</v>
       </c>
@@ -8556,8 +8704,28 @@
         <f>(C88/B97)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:20">
+      <c r="Q88">
+        <v>1.125</v>
+      </c>
+      <c r="R88">
+        <v>15</v>
+      </c>
+      <c r="S88">
+        <v>0</v>
+      </c>
+      <c r="T88">
+        <v>30</v>
+      </c>
+      <c r="W88">
+        <f>(S88/(S88+S98))</f>
+        <v>0</v>
+      </c>
+      <c r="X88">
+        <f>(S97/(S97+S88))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24">
       <c r="A89">
         <v>20</v>
       </c>
@@ -8578,8 +8746,28 @@
         <f>(C89/B97)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:20">
+      <c r="Q89">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R89">
+        <v>20</v>
+      </c>
+      <c r="S89">
+        <v>54</v>
+      </c>
+      <c r="T89">
+        <v>11</v>
+      </c>
+      <c r="W89">
+        <f>(S89/(S89+S98))</f>
+        <v>1.6158782178419287E-5</v>
+      </c>
+      <c r="X89">
+        <f>(S97/(S97+S89))</f>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24">
       <c r="A90">
         <v>25</v>
       </c>
@@ -8597,8 +8785,28 @@
         <f>(C90/B97)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:20">
+      <c r="Q90">
+        <v>1.075</v>
+      </c>
+      <c r="R90">
+        <v>25</v>
+      </c>
+      <c r="S90">
+        <v>356</v>
+      </c>
+      <c r="T90">
+        <v>5</v>
+      </c>
+      <c r="W90">
+        <f>(S90/(S90+S98))</f>
+        <v>1.0651864165991949E-4</v>
+      </c>
+      <c r="X90">
+        <f>(S97/(S97+S90))</f>
+        <v>7.7720207253886009E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24">
       <c r="A91">
         <v>30</v>
       </c>
@@ -8619,8 +8827,28 @@
         <f>(C91/B97)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:20">
+      <c r="Q91">
+        <v>1.05</v>
+      </c>
+      <c r="R91">
+        <v>30</v>
+      </c>
+      <c r="S91">
+        <v>701</v>
+      </c>
+      <c r="T91">
+        <v>4</v>
+      </c>
+      <c r="W91">
+        <f>(S91/(S91+S98))</f>
+        <v>2.0972432769291572E-4</v>
+      </c>
+      <c r="X91">
+        <f>(S97/(S97+S91))</f>
+        <v>4.1039671682626538E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24">
       <c r="A92">
         <v>35</v>
       </c>
@@ -8641,8 +8869,28 @@
         <f>(C92/B97)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:20">
+      <c r="Q92">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="R92">
+        <v>35</v>
+      </c>
+      <c r="S92">
+        <v>1164</v>
+      </c>
+      <c r="T92">
+        <v>2</v>
+      </c>
+      <c r="W92">
+        <f>(S92/(S92+S98))</f>
+        <v>3.4819587274218607E-4</v>
+      </c>
+      <c r="X92">
+        <f>(S97/(S97+S92))</f>
+        <v>2.5125628140703519E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24">
       <c r="A93">
         <v>40</v>
       </c>
@@ -8663,8 +8911,28 @@
         <f>(C93/B97)</f>
         <v>3.3333333333333333E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:20">
+      <c r="Q93">
+        <v>1</v>
+      </c>
+      <c r="R93">
+        <v>40</v>
+      </c>
+      <c r="S93">
+        <v>1583</v>
+      </c>
+      <c r="T93">
+        <v>2</v>
+      </c>
+      <c r="W93">
+        <f>(S95/(S95+S98))</f>
+        <v>6.4235794409571965E-4</v>
+      </c>
+      <c r="X93">
+        <f>(S97/(S97+S95))</f>
+        <v>1.3774104683195593E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24">
       <c r="A94">
         <v>45</v>
       </c>
@@ -8685,8 +8953,28 @@
         <f>(C94/B97)</f>
         <v>3.3333333333333333E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:20">
+      <c r="Q94">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R94">
+        <v>45</v>
+      </c>
+      <c r="S94">
+        <v>1758</v>
+      </c>
+      <c r="T94">
+        <v>2</v>
+      </c>
+      <c r="W94">
+        <f>(S95/(S95+S98))</f>
+        <v>6.4235794409571965E-4</v>
+      </c>
+      <c r="X94">
+        <f>(S97/(S97+S95))</f>
+        <v>1.3774104683195593E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24">
       <c r="A95">
         <v>50</v>
       </c>
@@ -8704,16 +8992,42 @@
         <f>(C95/B97)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="Q95">
+        <v>0.95</v>
+      </c>
+      <c r="R95">
+        <v>50</v>
+      </c>
+      <c r="S95">
+        <v>2148</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+      <c r="W95">
+        <f>(S95/(S95+S98))</f>
+        <v>6.4235794409571965E-4</v>
+      </c>
+      <c r="X95">
+        <f>(S97/(S97+S95))</f>
+        <v>1.3774104683195593E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B97">
         <v>30</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="R97" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S97">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" s="3" t="s">
         <v>77</v>
       </c>
@@ -8723,8 +9037,17 @@
       <c r="C98">
         <v>3341782</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="R98" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S98">
+        <v>3341782</v>
+      </c>
+      <c r="T98">
+        <v>24506406</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" s="16"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -8736,7 +9059,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="8"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:20">
       <c r="A100" s="16"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -8748,7 +9071,7 @@
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:20">
       <c r="A101" s="16"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
@@ -8760,7 +9083,7 @@
       <c r="I101" s="8"/>
       <c r="J101" s="8"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:20">
       <c r="A102" s="16"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -8772,7 +9095,7 @@
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:20">
       <c r="A103" s="16"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -8784,7 +9107,7 @@
       <c r="I103" s="8"/>
       <c r="J103" s="8"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:20">
       <c r="A104" s="16"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -8796,7 +9119,7 @@
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:20">
       <c r="A105" s="16"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -8808,7 +9131,7 @@
       <c r="I105" s="8"/>
       <c r="J105" s="8"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:20">
       <c r="A106" s="16"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -8820,7 +9143,7 @@
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:20">
       <c r="A107" s="16"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -8832,7 +9155,7 @@
       <c r="I107" s="8"/>
       <c r="J107" s="8"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:20">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -8844,7 +9167,7 @@
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:20">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
@@ -8856,7 +9179,7 @@
       <c r="I109" s="8"/>
       <c r="J109" s="8"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:20">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
@@ -8868,7 +9191,7 @@
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:20">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>

</xml_diff>